<commit_message>
Minor Updates in Chapter 2,4,5 an 8
</commit_message>
<xml_diff>
--- a/Chapter2/Hadoop-Cluster-Sizing-Calculator.xlsx
+++ b/Chapter2/Hadoop-Cluster-Sizing-Calculator.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hrishi\Personal\Hadoop3-book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hrishi\Personal\Hadoop3-book\source\git\Chapter2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{445B8895-2638-4D4F-AE9E-36D19EE85B12}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="0" windowWidth="23055" windowHeight="9795" activeTab="1"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="23055" windowHeight="9795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sizing Computation" sheetId="1" r:id="rId1"/>
     <sheet name="Hadoop Cluster Sizing" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>Data Source</t>
   </si>
@@ -168,9 +169,6 @@
     <t>Particular</t>
   </si>
   <si>
-    <t>Hadoop Data Cluster Size (A x B x C / (1-D))</t>
-  </si>
-  <si>
     <t>Non HDFS Storage Space in GBs</t>
   </si>
   <si>
@@ -184,12 +182,27 @@
   </si>
   <si>
     <t>Overall Storage</t>
+  </si>
+  <si>
+    <t>Hadoop Data Cluster Size (A x B x C / (1-D)) for Hadoop 1.X, 2.X</t>
+  </si>
+  <si>
+    <t>Hadoop 1.X, Hadoop 2.X</t>
+  </si>
+  <si>
+    <t>Hadoop 3.x</t>
+  </si>
+  <si>
+    <t>Considered for Erasure coding</t>
+  </si>
+  <si>
+    <t>Hadoop Data Cluster Size ((A x B) + (AxBx(C-1))*60%) / (1-D)) for Hadoop 3.X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -268,13 +281,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -294,6 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -315,7 +340,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -631,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -652,20 +679,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="J2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="J2" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="2:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -949,22 +976,22 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="8">
         <f>ROUND(SUM(G4:G13),0)</f>
         <v>1000031</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="9">
         <f>ROUND(G14/(1000*1000),2)</f>
         <v>1</v>
@@ -985,12 +1012,12 @@
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="J17" s="2" t="s">
         <v>22</v>
       </c>
@@ -999,11 +1026,11 @@
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="2">
         <v>1.5</v>
       </c>
@@ -1016,11 +1043,11 @@
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="5">
         <v>0.1</v>
       </c>
@@ -1033,11 +1060,11 @@
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="1">
         <f>ROUND(G18*(1+G19),2)</f>
         <v>1.65</v>
@@ -1051,22 +1078,22 @@
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="1">
         <f>G15</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="9">
         <f>SUM(G20:G21)</f>
         <v>2.65</v>
@@ -1086,10 +1113,10 @@
     <mergeCell ref="D19:F19"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C13" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$J$5:$J$11</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$J$16:$J$20</formula1>
     </dataValidation>
   </dataValidations>
@@ -1099,16 +1126,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="C2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
@@ -1130,7 +1157,7 @@
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2">
         <f>ROUND(D3*E4,2)</f>
@@ -1142,7 +1169,7 @@
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2">
         <f>ROUND(D3*E5,2)</f>
@@ -1154,7 +1181,7 @@
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="9">
         <f>SUM(D3:D5)</f>
@@ -1206,42 +1233,102 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="20">
+      <c r="C15" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="13">
         <f>(D10*D11*D12)/(1-D13)</f>
         <v>8.2200000000000006</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2">
+        <f>D16*E17</f>
+        <v>1.2330000000000001</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="2">
-        <f>D15*E16</f>
-        <v>1.2330000000000001</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="D18" s="3">
+        <f>ROUND(SUM(D15:D17),2)</f>
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="13">
+        <f>(D10*D11+((D10*D11)*(D12-1)*F21))/(1-D13)</f>
+        <v>6.0280000000000014</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2">
+        <f>D21*E22</f>
+        <v>0.90420000000000011</v>
+      </c>
+      <c r="E22" s="5">
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="3">
-        <f>ROUND(SUM(D15:D16),2)</f>
-        <v>9.4499999999999993</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3">
+        <f>ROUND(SUM(D20:D22),2)</f>
+        <v>6.93</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C20:E20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>